<commit_message>
Eeldusgraafis kriitilised teed korda + 3 näitegraafi.
</commit_message>
<xml_diff>
--- a/Algoritmide_omadused.xlsx
+++ b/Algoritmide_omadused.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hiie\Bakatöö\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hiie\Bakatöö\Repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -727,7 +727,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -986,7 +986,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>18</v>

</xml_diff>